<commit_message>
Updates to documentation tables
</commit_message>
<xml_diff>
--- a/docs/documentation_tables.xlsx
+++ b/docs/documentation_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\Creel_Analysis_Dev\CreelPointEstimate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/evan_booher_dfw_wa_gov/Documents/code/CreelPointEstimate/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D31D3C-95DD-4F65-A00B-3DC644941256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{06BDCB52-A10A-4652-9501-BAA58E581D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0398F24-454D-43F9-98DD-7ECDBFDE1231}"/>
   <bookViews>
-    <workbookView xWindow="-27555" yWindow="1020" windowWidth="26640" windowHeight="14520" firstSheet="1" activeTab="5" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
+    <workbookView xWindow="3825" yWindow="1065" windowWidth="22260" windowHeight="11910" firstSheet="3" activeTab="7" xr2:uid="{D87A213F-20EA-453F-96F1-E2F9D588DE08}"/>
   </bookViews>
   <sheets>
     <sheet name="design_stratification" sheetId="7" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="dwg_summ_interview" sheetId="4" r:id="rId4"/>
     <sheet name="dwg_summ_effort_index" sheetId="6" r:id="rId5"/>
     <sheet name="dwg_summ_effort_census" sheetId="5" r:id="rId6"/>
-    <sheet name="PE_output" sheetId="3" r:id="rId7"/>
+    <sheet name="PE_effort" sheetId="3" r:id="rId7"/>
+    <sheet name="PE_catch" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
   <si>
     <t>Data is stored in the creel database and accessible from data.wa.gov</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Primary key for interview table</t>
   </si>
   <si>
-    <t xml:space="preserve">Index value corresponding to the section (fishing location or interview location) where an interview occurred </t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -280,13 +277,118 @@
     <t>bank, boat</t>
   </si>
   <si>
-    <t>Specification of variable to group days within a week</t>
-  </si>
-  <si>
     <t>Specification of variable used to group n days of observations</t>
   </si>
   <si>
     <t>varies by estimation method; daily, week, month, "duration"</t>
+  </si>
+  <si>
+    <t>Index value representing the number of distinct index effort counts within a day at a given location</t>
+  </si>
+  <si>
+    <t>Category defining what was counted</t>
+  </si>
+  <si>
+    <t>Integer value for quanity of count_type observed</t>
+  </si>
+  <si>
+    <t>Indicator if the event was a tie-in survey, which typically consists of effort counts over larger sections than typical index counts and no interviews</t>
+  </si>
+  <si>
+    <t>Integer value for quanity of angler_final category observed</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>DayType</t>
+  </si>
+  <si>
+    <t>n_obs</t>
+  </si>
+  <si>
+    <t>ang_hrs_mean</t>
+  </si>
+  <si>
+    <t>ang_hrs_var</t>
+  </si>
+  <si>
+    <t>N_days_open</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>est</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>l95</t>
+  </si>
+  <si>
+    <t>u95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index value corresponding to the section where an interview occurred </t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification of the spatial domain used to aggregate observations from individual survey locations. A section contains one or more sites where effort counts and interviews occur. </t>
+  </si>
+  <si>
+    <t>each fishery project specifies the sites and corresponding sections which define the fishery area</t>
+  </si>
+  <si>
+    <t>Categorical variable used to aggregate days within a week</t>
+  </si>
+  <si>
+    <t>The number of observations (days) within specified strata (section_num, period, day_type, angler_final) available to calculate the sample mean</t>
+  </si>
+  <si>
+    <t>Index value corresponding to the time period in which aggregated observations occurred</t>
+  </si>
+  <si>
+    <t>Daily mean effort in units of angler hours from observed days within a straum (sample mean)</t>
+  </si>
+  <si>
+    <t>Daily variance of effort from observed days within a stratum (sample variance)</t>
+  </si>
+  <si>
+    <t>The number of days that the fishery was open for legal fishing within a stratum, representing the population total to which the sample mean is expanded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degrees of freedom; the number of independent observations used to calcuate the estimate </t>
+  </si>
+  <si>
+    <t>The expanded estimate of effort for the stratum, where ang_hrs_mean is multiplied by N_days_open</t>
+  </si>
+  <si>
+    <t>Variance the stratum estimate</t>
+  </si>
+  <si>
+    <t>lower 95% confidence interval using the student t distribution</t>
+  </si>
+  <si>
+    <t>upper 95% confidence interval using the student t distribution</t>
+  </si>
+  <si>
+    <t>catch_est_mean</t>
+  </si>
+  <si>
+    <t>catch_est_var</t>
+  </si>
+  <si>
+    <t>categorical value for corresponding catch group to which estimate is associated</t>
+  </si>
+  <si>
+    <t>Daily mean catch (count of fish) from observed days within a straum (sample mean)</t>
+  </si>
+  <si>
+    <t>The expanded estimate of catch for the stratum, where catch_est_mean is multiplied by N_days_open</t>
   </si>
 </sst>
 </file>
@@ -659,17 +761,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8884888-2887-40E7-9CF4-425C1A207D31}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="136.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="160.42578125" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,40 +782,51 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +1049,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +1079,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,7 +1087,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,7 +1095,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +1103,7 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -998,7 +1111,7 @@
         <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +1119,7 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,7 +1127,7 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1135,7 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,7 +1143,7 @@
         <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1038,7 +1151,7 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1159,7 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1167,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1175,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,7 +1183,7 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1191,7 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1092,13 +1205,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="97.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1113,25 +1226,40 @@
       <c r="A2" t="s">
         <v>35</v>
       </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1144,14 +1272,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12605542-A2C1-4215-B756-E02144100F73}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="131.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,35 +1294,56 @@
       <c r="A2" t="s">
         <v>35</v>
       </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1205,16 +1354,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75E7F5D-D201-4287-A106-3CF707809EE2}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="2" max="2" width="147.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1225,8 +1374,251 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA93150C-F2EF-4B20-BF9C-B8E1EA328C72}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="138.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>